<commit_message>
updated to account for lakes with multiple deep spots
</commit_message>
<xml_diff>
--- a/data/lookup.xlsx
+++ b/data/lookup.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\WD-Watershed\Monitoring\Volunteer\VLAP\Data Reporting\Annual reports\2025\VLAP-Annual-Reports\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33483E0-3205-4338-B56B-59025FAEF76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D301BE57-A371-4865-81CE-CED4A5595704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34620" yWindow="1035" windowWidth="21600" windowHeight="11295" xr2:uid="{3A1B09BE-8A81-46D6-B56A-F8CD7FE6F52C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3A1B09BE-8A81-46D6-B56A-F8CD7FE6F52C}"/>
   </bookViews>
   <sheets>
     <sheet name="lookup" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">lookup!$A$1:$E$109</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="126">
   <si>
     <t>lake</t>
   </si>
@@ -212,27 +215,15 @@
     <t>PAWNOTND</t>
   </si>
   <si>
-    <t>#08 FERNALDS A</t>
-  </si>
-  <si>
     <t>PAWNNOTF1</t>
   </si>
   <si>
-    <t>#04 MOUNTAIN BK</t>
-  </si>
-  <si>
     <t>PAWSNOTM</t>
   </si>
   <si>
-    <t>#14 ROUND POND BK</t>
-  </si>
-  <si>
     <t>PAWNNOTR</t>
   </si>
   <si>
-    <t>#11 BACK CREEK B</t>
-  </si>
-  <si>
     <t>PAWNNOTB</t>
   </si>
   <si>
@@ -333,6 +324,96 @@
   </si>
   <si>
     <t>MONKEY POND CULVERT</t>
+  </si>
+  <si>
+    <t>COBWINARM</t>
+  </si>
+  <si>
+    <t>ARMSTRONG</t>
+  </si>
+  <si>
+    <t>CONNIE'S BROOK AT 111</t>
+  </si>
+  <si>
+    <t>COBWINCB111</t>
+  </si>
+  <si>
+    <t>DINSMORE WEST</t>
+  </si>
+  <si>
+    <t>COBWINDW</t>
+  </si>
+  <si>
+    <t>COBWINFR</t>
+  </si>
+  <si>
+    <t>FOSSA RD INLET</t>
+  </si>
+  <si>
+    <t>COBWINWR</t>
+  </si>
+  <si>
+    <t>COBWINMESS</t>
+  </si>
+  <si>
+    <t>COBWINMS</t>
+  </si>
+  <si>
+    <t>COBWINMI</t>
+  </si>
+  <si>
+    <t>MESS</t>
+  </si>
+  <si>
+    <t>MUELLER STREAM</t>
+  </si>
+  <si>
+    <t>WALKEY RD</t>
+  </si>
+  <si>
+    <t>MONSON INLET</t>
+  </si>
+  <si>
+    <t>PARK RD</t>
+  </si>
+  <si>
+    <t>GRTKING</t>
+  </si>
+  <si>
+    <t>PAWNNOTW</t>
+  </si>
+  <si>
+    <t>PAWNNOTF2</t>
+  </si>
+  <si>
+    <t>PAWNNOTF3</t>
+  </si>
+  <si>
+    <t>ROUND PD BROOK</t>
+  </si>
+  <si>
+    <t>NORTH DEEP SPOT</t>
+  </si>
+  <si>
+    <t>BACK CREEK B</t>
+  </si>
+  <si>
+    <t>SOUTH DEEP SPOT</t>
+  </si>
+  <si>
+    <t>WHITE GROVE BROOK</t>
+  </si>
+  <si>
+    <t>FUNDY BROOK</t>
+  </si>
+  <si>
+    <t>MOUNTAIN BROOK</t>
+  </si>
+  <si>
+    <t>FERNALDS A</t>
+  </si>
+  <si>
+    <t>FERNALDS B</t>
   </si>
 </sst>
 </file>
@@ -816,8 +897,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1193,10 +1275,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE83FF0B-EFA6-43E5-B9C8-616EF3C472BB}">
-  <dimension ref="A1:C96"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104:XFD104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,150 +1301,150 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>103</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>108</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
         <v>21</v>
@@ -1373,164 +1455,164 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>111</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
         <v>29</v>
@@ -1538,354 +1620,354 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B31" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C33" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B34" t="s">
         <v>21</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B35" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B36" t="s">
-        <v>3</v>
+        <v>112</v>
       </c>
       <c r="C36" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B37" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C37" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B38" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C38" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B39" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B40" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C40" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B41" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B42" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C42" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B43" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="C44" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C45" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B47" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C47" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="C48" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B49" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C49" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B50" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B51" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C51" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B52" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C52" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B53" t="s">
-        <v>3</v>
+        <v>119</v>
       </c>
       <c r="C53" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B54" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B55" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C55" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B56" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="C56" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B57" t="s">
-        <v>20</v>
+        <v>125</v>
       </c>
       <c r="C57" t="s">
-        <v>48</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B58" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="C58" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B59" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C59" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B60" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C60" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B61" t="s">
-        <v>21</v>
+        <v>123</v>
       </c>
       <c r="C61" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B62" t="s">
-        <v>22</v>
+        <v>118</v>
       </c>
       <c r="C62" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1893,10 +1975,10 @@
         <v>93</v>
       </c>
       <c r="B63" t="s">
-        <v>3</v>
+        <v>117</v>
       </c>
       <c r="C63" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1904,365 +1986,456 @@
         <v>93</v>
       </c>
       <c r="B64" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="C64" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B65" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B66" t="s">
         <v>22</v>
       </c>
       <c r="C66" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B67" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C67" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B68" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C68" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B69" t="s">
-        <v>21</v>
+        <v>120</v>
       </c>
       <c r="C69" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>94</v>
-      </c>
-      <c r="B70" t="s">
-        <v>22</v>
-      </c>
-      <c r="C70" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D70" s="1"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B71" t="s">
         <v>3</v>
       </c>
       <c r="C71" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D72" s="1"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>87</v>
+      </c>
+      <c r="B73" t="s">
+        <v>22</v>
+      </c>
+      <c r="C73" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>87</v>
+      </c>
+      <c r="B74" t="s">
+        <v>20</v>
+      </c>
+      <c r="C74" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>87</v>
+      </c>
+      <c r="B75" t="s">
+        <v>52</v>
+      </c>
+      <c r="C75" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D76" s="1"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>87</v>
+      </c>
+      <c r="B77" t="s">
+        <v>21</v>
+      </c>
+      <c r="C77" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>87</v>
+      </c>
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>87</v>
+      </c>
+      <c r="B79" t="s">
+        <v>49</v>
+      </c>
+      <c r="C79" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>87</v>
+      </c>
+      <c r="B80" t="s">
+        <v>28</v>
+      </c>
+      <c r="C80" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D81" s="1"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D82" s="1"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D83" s="1"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D84" s="1"/>
+    </row>
+    <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D85" s="1"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>88</v>
+      </c>
+      <c r="B86" t="s">
+        <v>3</v>
+      </c>
+      <c r="C86" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>88</v>
+      </c>
+      <c r="B87" t="s">
+        <v>22</v>
+      </c>
+      <c r="C87" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>88</v>
+      </c>
+      <c r="B88" t="s">
+        <v>20</v>
+      </c>
+      <c r="C88" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>21</v>
+      </c>
+      <c r="C89" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D90" s="1"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>88</v>
+      </c>
+      <c r="B91" t="s">
+        <v>28</v>
+      </c>
+      <c r="C91" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D92" s="1"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>89</v>
+      </c>
+      <c r="B93" t="s">
+        <v>3</v>
+      </c>
+      <c r="C93" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>89</v>
+      </c>
+      <c r="B94" t="s">
+        <v>22</v>
+      </c>
+      <c r="C94" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>89</v>
+      </c>
+      <c r="B95" t="s">
+        <v>20</v>
+      </c>
+      <c r="C95" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>89</v>
+      </c>
+      <c r="B96" t="s">
+        <v>21</v>
+      </c>
+      <c r="C96" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>91</v>
+      </c>
+      <c r="B97" t="s">
+        <v>3</v>
+      </c>
+      <c r="C97" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>95</v>
-      </c>
-      <c r="B72" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>91</v>
+      </c>
+      <c r="B98" t="s">
+        <v>22</v>
+      </c>
+      <c r="C98" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>91</v>
+      </c>
+      <c r="B99" t="s">
         <v>20</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C99" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>95</v>
-      </c>
-      <c r="B73" t="s">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>91</v>
+      </c>
+      <c r="B100" t="s">
         <v>21</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C100" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>95</v>
-      </c>
-      <c r="B74" t="s">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>90</v>
+      </c>
+      <c r="B101" t="s">
+        <v>3</v>
+      </c>
+      <c r="C101" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>90</v>
+      </c>
+      <c r="B102" t="s">
         <v>22</v>
       </c>
-      <c r="C74" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>96</v>
-      </c>
-      <c r="B75" t="s">
-        <v>3</v>
-      </c>
-      <c r="C75" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>97</v>
-      </c>
-      <c r="B76" t="s">
-        <v>3</v>
-      </c>
-      <c r="C76" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>97</v>
-      </c>
-      <c r="B77" t="s">
-        <v>59</v>
-      </c>
-      <c r="C77" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>97</v>
-      </c>
-      <c r="B78" t="s">
-        <v>61</v>
-      </c>
-      <c r="C78" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>97</v>
-      </c>
-      <c r="B79" t="s">
-        <v>63</v>
-      </c>
-      <c r="C79" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>97</v>
-      </c>
-      <c r="B80" t="s">
-        <v>65</v>
-      </c>
-      <c r="C80" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>96</v>
-      </c>
-      <c r="B81" t="s">
+      <c r="C102" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>90</v>
+      </c>
+      <c r="B103" t="s">
         <v>20</v>
       </c>
-      <c r="C81" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>96</v>
-      </c>
-      <c r="B82" t="s">
-        <v>21</v>
-      </c>
-      <c r="C82" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>96</v>
-      </c>
-      <c r="B83" t="s">
-        <v>22</v>
-      </c>
-      <c r="C83" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>97</v>
-      </c>
-      <c r="B84" t="s">
-        <v>20</v>
-      </c>
-      <c r="C84" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>97</v>
-      </c>
-      <c r="B85" t="s">
-        <v>21</v>
-      </c>
-      <c r="C85" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>97</v>
-      </c>
-      <c r="B86" t="s">
-        <v>22</v>
-      </c>
-      <c r="C86" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>92</v>
-      </c>
-      <c r="B87" t="s">
-        <v>67</v>
-      </c>
-      <c r="C87" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>92</v>
-      </c>
-      <c r="B88" t="s">
-        <v>69</v>
-      </c>
-      <c r="C88" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>91</v>
-      </c>
-      <c r="B89" t="s">
-        <v>71</v>
-      </c>
-      <c r="C89" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>91</v>
-      </c>
-      <c r="B90" t="s">
-        <v>73</v>
-      </c>
-      <c r="C90" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>91</v>
-      </c>
-      <c r="B91" t="s">
-        <v>75</v>
-      </c>
-      <c r="C91" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>91</v>
-      </c>
-      <c r="B92" t="s">
-        <v>77</v>
-      </c>
-      <c r="C92" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>91</v>
-      </c>
-      <c r="B93" t="s">
-        <v>79</v>
-      </c>
-      <c r="C93" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>91</v>
-      </c>
-      <c r="B94" t="s">
-        <v>81</v>
-      </c>
-      <c r="C94" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>92</v>
-      </c>
-      <c r="B95" t="s">
-        <v>83</v>
-      </c>
-      <c r="C95" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>92</v>
-      </c>
-      <c r="B96" t="s">
-        <v>99</v>
-      </c>
-      <c r="C96" t="s">
-        <v>98</v>
+      <c r="C103" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D111">
+    <sortCondition ref="A2:A111"/>
+    <sortCondition ref="B2:B111"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed the LAKEMAP overwriting problem
</commit_message>
<xml_diff>
--- a/data/lookup.xlsx
+++ b/data/lookup.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\WD-Watershed\Monitoring\Volunteer\VLAP\Data Reporting\Annual reports\2025\VLAP-Annual-Reports\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D301BE57-A371-4865-81CE-CED4A5595704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AC21FF-3870-42CD-9918-6285ED0A8925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3A1B09BE-8A81-46D6-B56A-F8CD7FE6F52C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3A1B09BE-8A81-46D6-B56A-F8CD7FE6F52C}"/>
   </bookViews>
   <sheets>
     <sheet name="lookup" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">lookup!$A$1:$E$109</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">lookup!$A$1:$E$91</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="175">
   <si>
     <t>lake</t>
   </si>
@@ -414,6 +414,153 @@
   </si>
   <si>
     <t>FERNALDS B</t>
+  </si>
+  <si>
+    <t>COBWINHC</t>
+  </si>
+  <si>
+    <t>COBWINCC</t>
+  </si>
+  <si>
+    <t>COBWINDE</t>
+  </si>
+  <si>
+    <t>COBWINBDD</t>
+  </si>
+  <si>
+    <t>HERONS COVE</t>
+  </si>
+  <si>
+    <t>CASTLETON CULVERT</t>
+  </si>
+  <si>
+    <t>DINSMORE EAST</t>
+  </si>
+  <si>
+    <t>BELOW DUNKIN DONTUS</t>
+  </si>
+  <si>
+    <t>COBWINCBW</t>
+  </si>
+  <si>
+    <t>COBWINCBCVS</t>
+  </si>
+  <si>
+    <t>CONNIES BROOK AT CVS</t>
+  </si>
+  <si>
+    <t>CONNIES BK WEST</t>
+  </si>
+  <si>
+    <t>COBBETTS POND, STN1</t>
+  </si>
+  <si>
+    <t>GRTKINB</t>
+  </si>
+  <si>
+    <t>BALL RD INLET</t>
+  </si>
+  <si>
+    <t>HIGSTDCB</t>
+  </si>
+  <si>
+    <t>HIGSTDP</t>
+  </si>
+  <si>
+    <t>HIGSTDRBT</t>
+  </si>
+  <si>
+    <t>HIGSTDKT</t>
+  </si>
+  <si>
+    <t>CARR BK ENTRANCE TO LAKE</t>
+  </si>
+  <si>
+    <t>PICKEREL COVE BROOK</t>
+  </si>
+  <si>
+    <t>RICE BROOK TRIB</t>
+  </si>
+  <si>
+    <t>KENNEDY BK TRIB</t>
+  </si>
+  <si>
+    <t>PAWNNOTDAM1</t>
+  </si>
+  <si>
+    <t>PAWNNOTDAM2</t>
+  </si>
+  <si>
+    <t>PAWNNOT18IR</t>
+  </si>
+  <si>
+    <t>PAWNNOTH</t>
+  </si>
+  <si>
+    <t>PAWNNOTNEC</t>
+  </si>
+  <si>
+    <t>PAWNNOTNEILS</t>
+  </si>
+  <si>
+    <t>DOLLOFF DAM</t>
+  </si>
+  <si>
+    <t>DROWNS DAM</t>
+  </si>
+  <si>
+    <t>18 INDIAN RD</t>
+  </si>
+  <si>
+    <t>HIGHLAND AVE</t>
+  </si>
+  <si>
+    <t>NORTHEAST COVE</t>
+  </si>
+  <si>
+    <t>NEILS COVE</t>
+  </si>
+  <si>
+    <t>WINPLACB</t>
+  </si>
+  <si>
+    <t>WINPLACW</t>
+  </si>
+  <si>
+    <t>WINTLACC</t>
+  </si>
+  <si>
+    <t>WINTLACGB</t>
+  </si>
+  <si>
+    <t>WINTLACGS</t>
+  </si>
+  <si>
+    <t>WINTLACM</t>
+  </si>
+  <si>
+    <t>WINPLACBCHI</t>
+  </si>
+  <si>
+    <t>BLACK BK</t>
+  </si>
+  <si>
+    <t>BEACH INLET</t>
+  </si>
+  <si>
+    <t>WINNIPESAUKEE R</t>
+  </si>
+  <si>
+    <t>COLLINS BK</t>
+  </si>
+  <si>
+    <t>GOV PARK BCH</t>
+  </si>
+  <si>
+    <t>GOV PARK STREAM</t>
+  </si>
+  <si>
+    <t>MILL BK</t>
   </si>
 </sst>
 </file>
@@ -899,7 +1046,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1275,17 +1422,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE83FF0B-EFA6-43E5-B9C8-616EF3C472BB}">
-  <dimension ref="A1:D103"/>
+  <dimension ref="A1:C127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104:XFD104"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H117" sqref="H117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1311,14 +1458,14 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
+      <c r="A3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1326,10 +1473,10 @@
         <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1337,10 +1484,10 @@
         <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1348,43 +1495,43 @@
         <v>82</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C7" t="s">
-        <v>99</v>
+      <c r="B7" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C8" t="s">
-        <v>101</v>
+      <c r="B8" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
+      <c r="B9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1392,21 +1539,21 @@
         <v>82</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
+      <c r="B11" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1414,10 +1561,10 @@
         <v>82</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1425,21 +1572,21 @@
         <v>82</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B14" t="s">
-        <v>108</v>
-      </c>
-      <c r="C14" t="s">
-        <v>105</v>
+      <c r="B14" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1447,10 +1594,10 @@
         <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1458,10 +1605,10 @@
         <v>82</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>107</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1469,10 +1616,10 @@
         <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1480,10 +1627,10 @@
         <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1491,21 +1638,21 @@
         <v>82</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>109</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
-        <v>110</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1513,7 +1660,7 @@
         <v>81</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -1524,7 +1671,7 @@
         <v>81</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -1535,7 +1682,7 @@
         <v>81</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -1543,90 +1690,90 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B26" t="s">
         <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
         <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B28" t="s">
         <v>21</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>83</v>
-      </c>
-      <c r="B31" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" t="s">
-        <v>29</v>
+      <c r="B31" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1634,10 +1781,10 @@
         <v>83</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>112</v>
       </c>
       <c r="C32" t="s">
-        <v>29</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1653,134 +1800,134 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C35" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B36" t="s">
-        <v>112</v>
+        <v>20</v>
       </c>
       <c r="C36" t="s">
-        <v>113</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B37" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C37" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B38" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C38" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B39" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B41" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C41" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C42" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B44" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C44" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C45" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1788,10 +1935,10 @@
         <v>86</v>
       </c>
       <c r="B46" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1799,21 +1946,21 @@
         <v>86</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C47" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B48" t="s">
-        <v>41</v>
-      </c>
-      <c r="C48" t="s">
-        <v>42</v>
+      <c r="B48" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1821,620 +1968,873 @@
         <v>86</v>
       </c>
       <c r="B49" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C49" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B50" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="C50" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>85</v>
-      </c>
-      <c r="B51" t="s">
-        <v>22</v>
-      </c>
-      <c r="C51" t="s">
-        <v>31</v>
+      <c r="A51" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B52" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C52" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B53" t="s">
-        <v>119</v>
+        <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B54" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C54" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B55" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C55" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B56" t="s">
-        <v>124</v>
+        <v>21</v>
       </c>
       <c r="C56" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>93</v>
-      </c>
-      <c r="B57" t="s">
-        <v>125</v>
-      </c>
-      <c r="C57" t="s">
-        <v>116</v>
+      <c r="A57" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B58" t="s">
-        <v>122</v>
+        <v>41</v>
       </c>
       <c r="C58" t="s">
-        <v>115</v>
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B59" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C59" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>93</v>
-      </c>
-      <c r="B60" t="s">
-        <v>21</v>
-      </c>
-      <c r="C60" t="s">
-        <v>58</v>
+      <c r="A60" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B61" t="s">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="C61" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B62" t="s">
-        <v>118</v>
+        <v>22</v>
       </c>
       <c r="C62" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>85</v>
+      </c>
+      <c r="B63" t="s">
+        <v>20</v>
+      </c>
+      <c r="C63" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>93</v>
+      </c>
+      <c r="B65" t="s">
+        <v>119</v>
+      </c>
+      <c r="C65" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>93</v>
+      </c>
+      <c r="B68" t="s">
+        <v>124</v>
+      </c>
+      <c r="C68" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>93</v>
+      </c>
+      <c r="B69" t="s">
+        <v>122</v>
+      </c>
+      <c r="C69" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>93</v>
+      </c>
+      <c r="B70" t="s">
+        <v>125</v>
+      </c>
+      <c r="C70" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>93</v>
+      </c>
+      <c r="B74" t="s">
         <v>117</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C74" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>93</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B75" t="s">
         <v>121</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C75" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>93</v>
+      </c>
+      <c r="B76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>93</v>
+      </c>
+      <c r="B77" t="s">
+        <v>22</v>
+      </c>
+      <c r="C77" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>93</v>
+      </c>
+      <c r="B78" t="s">
+        <v>20</v>
+      </c>
+      <c r="C78" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>93</v>
+      </c>
+      <c r="B79" t="s">
+        <v>21</v>
+      </c>
+      <c r="C79" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>93</v>
+      </c>
+      <c r="B80" t="s">
+        <v>118</v>
+      </c>
+      <c r="C80" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>92</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B81" t="s">
         <v>3</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C81" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>92</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B82" t="s">
         <v>22</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C82" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>92</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B83" t="s">
         <v>20</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C83" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>92</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B84" t="s">
         <v>21</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C84" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>92</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B85" t="s">
         <v>120</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C85" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D70" s="1"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>87</v>
-      </c>
-      <c r="B71" t="s">
-        <v>3</v>
-      </c>
-      <c r="C71" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D72" s="1"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>87</v>
-      </c>
-      <c r="B73" t="s">
-        <v>22</v>
-      </c>
-      <c r="C73" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>87</v>
-      </c>
-      <c r="B74" t="s">
-        <v>20</v>
-      </c>
-      <c r="C74" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>87</v>
-      </c>
-      <c r="B75" t="s">
-        <v>52</v>
-      </c>
-      <c r="C75" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D76" s="1"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>87</v>
-      </c>
-      <c r="B77" t="s">
-        <v>21</v>
-      </c>
-      <c r="C77" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>87</v>
-      </c>
-      <c r="B78" t="s">
-        <v>8</v>
-      </c>
-      <c r="C78" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>87</v>
-      </c>
-      <c r="B79" t="s">
-        <v>49</v>
-      </c>
-      <c r="C79" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>87</v>
-      </c>
-      <c r="B80" t="s">
-        <v>28</v>
-      </c>
-      <c r="C80" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D81" s="1"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D82" s="1"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D83" s="1"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D84" s="1"/>
-    </row>
-    <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D85" s="1"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B86" t="s">
-        <v>3</v>
+        <v>123</v>
       </c>
       <c r="C86" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>88</v>
       </c>
       <c r="B87" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="C87" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="C88" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="C89" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D90" s="1"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>87</v>
+      </c>
+      <c r="B90" t="s">
+        <v>73</v>
+      </c>
+      <c r="C90" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B91" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="C91" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D92" s="1"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>87</v>
+      </c>
+      <c r="B92" t="s">
+        <v>75</v>
+      </c>
+      <c r="C92" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B93" t="s">
+        <v>69</v>
+      </c>
+      <c r="C93" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>87</v>
+      </c>
+      <c r="B94" t="s">
+        <v>67</v>
+      </c>
+      <c r="C94" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>87</v>
+      </c>
+      <c r="B95" t="s">
+        <v>52</v>
+      </c>
+      <c r="C95" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>87</v>
+      </c>
+      <c r="B96" t="s">
         <v>3</v>
       </c>
-      <c r="C93" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>89</v>
-      </c>
-      <c r="B94" t="s">
-        <v>22</v>
-      </c>
-      <c r="C94" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>89</v>
-      </c>
-      <c r="B95" t="s">
-        <v>20</v>
-      </c>
-      <c r="C95" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>89</v>
-      </c>
-      <c r="B96" t="s">
-        <v>21</v>
-      </c>
       <c r="C96" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B97" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C97" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B98" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C98" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B99" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C99" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B100" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C100" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B101" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="C101" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B102" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C102" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>87</v>
+      </c>
+      <c r="B103" t="s">
+        <v>49</v>
+      </c>
+      <c r="C103" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>88</v>
+      </c>
+      <c r="B104" t="s">
+        <v>79</v>
+      </c>
+      <c r="C104" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>88</v>
+      </c>
+      <c r="B105" t="s">
+        <v>3</v>
+      </c>
+      <c r="C105" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>88</v>
+      </c>
+      <c r="B106" t="s">
+        <v>22</v>
+      </c>
+      <c r="C106" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>88</v>
+      </c>
+      <c r="B107" t="s">
+        <v>20</v>
+      </c>
+      <c r="C107" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>88</v>
+      </c>
+      <c r="B108" t="s">
+        <v>21</v>
+      </c>
+      <c r="C108" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>88</v>
+      </c>
+      <c r="B109" t="s">
+        <v>28</v>
+      </c>
+      <c r="C109" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>89</v>
+      </c>
+      <c r="B110" t="s">
+        <v>3</v>
+      </c>
+      <c r="C110" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>89</v>
+      </c>
+      <c r="B111" t="s">
+        <v>22</v>
+      </c>
+      <c r="C111" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>89</v>
+      </c>
+      <c r="B112" t="s">
+        <v>20</v>
+      </c>
+      <c r="C112" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>89</v>
+      </c>
+      <c r="B113" t="s">
+        <v>21</v>
+      </c>
+      <c r="C113" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>91</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>91</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>91</v>
+      </c>
+      <c r="B116" t="s">
+        <v>3</v>
+      </c>
+      <c r="C116" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>91</v>
+      </c>
+      <c r="B117" t="s">
+        <v>22</v>
+      </c>
+      <c r="C117" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>91</v>
+      </c>
+      <c r="B118" t="s">
+        <v>20</v>
+      </c>
+      <c r="C118" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>91</v>
+      </c>
+      <c r="B119" t="s">
+        <v>21</v>
+      </c>
+      <c r="C119" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>91</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>90</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B121" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>90</v>
+      </c>
+      <c r="B122" t="s">
+        <v>3</v>
+      </c>
+      <c r="C122" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>90</v>
+      </c>
+      <c r="B123" t="s">
+        <v>22</v>
+      </c>
+      <c r="C123" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>90</v>
+      </c>
+      <c r="B124" t="s">
         <v>20</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C124" t="s">
         <v>55</v>
       </c>
     </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>90</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>90</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>90</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D111">
-    <sortCondition ref="A2:A111"/>
-    <sortCondition ref="B2:B111"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C160">
+    <sortCondition ref="C2:C160"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>